<commit_message>
GOIDA GOIDA 2 2
</commit_message>
<xml_diff>
--- a/bot/db/applicants.xlsx
+++ b/bot/db/applicants.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,33 +434,162 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Как вас зовут?</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Какой ваш любимый цвет?</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Какой ваш любимый фильм?</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Какой ваш любимый вид спорта?</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sda</t>
+          <t>LowIQMulti</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>denis</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Красный</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>UIIUII</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Баскетбол</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Синий</t>
+          <t>LowIQMulti</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ty</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Красный</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ty</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Баскетбол</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dsa</t>
+          <t>drus1k0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Синий</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Hohlo</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Футбол</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
+        <is>
+          <t>LowIQMulti</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Егор</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Красный</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>неет</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Баскетбол</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>GasBillt</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Dis</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Синий</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tg</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Футбол</t>
         </is>

</xml_diff>